<commit_message>
Generation and Storage Update
</commit_message>
<xml_diff>
--- a/Batt_Temp_Month.xlsx
+++ b/Batt_Temp_Month.xlsx
@@ -678,16 +678,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>30.17910891089108</v>
+        <v>30.36894366197182</v>
       </c>
       <c r="C13">
-        <v>27.28118811881188</v>
+        <v>26.61549295774649</v>
       </c>
       <c r="D13">
-        <v>27.28118811881188</v>
+        <v>26.61549295774649</v>
       </c>
       <c r="E13">
-        <v>29.24871287128713</v>
+        <v>29.13345070422535</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -695,16 +695,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>29.84014084507041</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>25.47957746478873</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>25.47957746478873</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>27.65450704225353</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -712,16 +712,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>27.40859154929578</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>23.47887323943662</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>23.47887323943662</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>25.25387323943661</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -729,16 +729,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>4967.880212765958</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>24.1372340425532</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>24.1372340425532</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>25.64478723404255</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>